<commit_message>
New option chain data and different minimize methods
</commit_message>
<xml_diff>
--- a/petr_options_chain_3.xlsx
+++ b/petr_options_chain_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.hun\Documents\repos\medium_interpolation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1734AD96-DBAB-4C2A-9413-224441A6E034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47C186C-A872-41F1-8B66-4A978A85907F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5828EF37-8FFC-474E-B380-CED8276F2316}"/>
+    <workbookView xWindow="-23010" yWindow="750" windowWidth="21600" windowHeight="15000" xr2:uid="{5828EF37-8FFC-474E-B380-CED8276F2316}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6256,8 +6256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB6F38C-C06D-4011-9266-3D021F228CA4}">
   <dimension ref="A1:T1925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="O101" sqref="O101"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add for on the scratch for running multiple simulations
</commit_message>
<xml_diff>
--- a/petr_options_chain_3.xlsx
+++ b/petr_options_chain_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.hun\Documents\repos\medium_interpolation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47C186C-A872-41F1-8B66-4A978A85907F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56FD035-54A4-4CB9-BE68-AA09FB530EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23010" yWindow="750" windowWidth="21600" windowHeight="15000" xr2:uid="{5828EF37-8FFC-474E-B380-CED8276F2316}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5828EF37-8FFC-474E-B380-CED8276F2316}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6256,8 +6278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB6F38C-C06D-4011-9266-3D021F228CA4}">
   <dimension ref="A1:T1925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9:P18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I871" sqref="I871"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6265,7 +6287,7 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6297,7 +6319,7 @@
         <v>1944</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6328,8 +6350,12 @@
       <c r="J2">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M2" t="str" cm="1">
+        <f t="array" ref="M2:M17">_xlfn.UNIQUE(G:G)</f>
+        <v>Expiry</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -6360,8 +6386,11 @@
       <c r="J3">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M3" t="str">
+        <v>24/10/2025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -6392,8 +6421,11 @@
       <c r="J4">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M4" t="str">
+        <v>31/10/2025</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -6424,8 +6456,11 @@
       <c r="J5">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>45849</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -6456,8 +6491,11 @@
       <c r="J6">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M6" t="str">
+        <v>14/11/2025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -6488,8 +6526,11 @@
       <c r="J7">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M7" t="str">
+        <v>21/11/2025</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -6520,8 +6561,11 @@
       <c r="J8">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M8" t="str">
+        <v>28/11/2025</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -6552,8 +6596,11 @@
       <c r="J9">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -6584,8 +6631,11 @@
       <c r="J10">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>46003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -6616,8 +6666,11 @@
       <c r="J11">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M11" t="str">
+        <v>19/12/2025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -6648,8 +6701,11 @@
       <c r="J12">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M12" t="str">
+        <v>26/12/2025</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -6680,8 +6736,11 @@
       <c r="J13">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M13" t="str">
+        <v>16/01/2026</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -6712,8 +6771,11 @@
       <c r="J14">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M14" t="str">
+        <v>20/02/2026</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -6744,8 +6806,11 @@
       <c r="J15">
         <v>29.73</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M15" t="str">
+        <v>20/03/2026</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -6775,6 +6840,9 @@
       </c>
       <c r="J16">
         <v>29.73</v>
+      </c>
+      <c r="M16" t="str">
+        <v>17/04/2026</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
@@ -6807,6 +6875,9 @@
       </c>
       <c r="J17">
         <v>29.73</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>